<commit_message>
code review competed - added rng seed - ready for data collection
</commit_message>
<xml_diff>
--- a/doc/carrefour_data_collection.xlsx
+++ b/doc/carrefour_data_collection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\the_carrefour\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\the_carrefour_pecsn\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A1CF32-1887-49D7-9149-D780D4BB647E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CBF8C0-AD51-4A7A-AFA2-C0ECF1A8679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2985" yWindow="3015" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="23">
   <si>
     <t>data collection at Carrefour San Giuliano Terme</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>AVG</t>
+  </si>
+  <si>
+    <t>PROCESSING TIME</t>
   </si>
 </sst>
 </file>
@@ -468,7 +471,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F4"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +619,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +760,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,62 +921,79 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{785EF536-0FBE-4240-A3CE-9D59537A6013}">
-  <dimension ref="A2:B16"/>
+  <dimension ref="A2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2">
         <v>51.74</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2">
+        <v>152.69999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>68.95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>99.45</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>141.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>16.649999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>91.46</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>92.38</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>44.29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -981,22 +1001,22 @@
         <v>66.930000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>4.08</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>21.78</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>34.92</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1004,12 +1024,12 @@
         <v>17.649999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>14.51</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>21</v>
       </c>

</xml_diff>